<commit_message>
data from input file (tooth and stent model)
</commit_message>
<xml_diff>
--- a/Projects/project2/viz/error.xlsx
+++ b/Projects/project2/viz/error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Documents\GitHub\ECS277\Projects\project2\viz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6BF4D8-8D5E-4AFB-AD2E-24936DD0CCFD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C873E1-D768-4B12-999C-873E0B7B9D6F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{9984D9AA-9010-4E22-858C-C2CD43C27DAF}"/>
   </bookViews>
@@ -954,7 +954,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.16485890643691198"/>
           <c:y val="0.39752246917963763"/>
-          <c:w val="0.13331713782237634"/>
+          <c:w val="0.17287023592503442"/>
           <c:h val="0.35704530536549556"/>
         </c:manualLayout>
       </c:layout>
@@ -1867,9 +1867,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14401518611470218"/>
-          <c:y val="0.24839136237724499"/>
-          <c:w val="0.13230525227486534"/>
+          <c:x val="0.14255024936085278"/>
+          <c:y val="0.20597797686237876"/>
+          <c:w val="0.16892842427656746"/>
           <c:h val="0.35704530536549556"/>
         </c:manualLayout>
       </c:layout>
@@ -5173,7 +5173,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.14401518611470218"/>
           <c:y val="0.24839136237724499"/>
-          <c:w val="0.13230525227486534"/>
+          <c:w val="0.17185828164557404"/>
           <c:h val="0.24835653261120949"/>
         </c:manualLayout>
       </c:layout>

</xml_diff>